<commit_message>
Database updated - addOperation controller
* Delete intermediate table user_administration
* user_id created in administrations
* addOperation added + Modal in front
</commit_message>
<xml_diff>
--- a/APP.xlsx
+++ b/APP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\DH\Adm-Presupuesto-Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DAB34B-5944-4BDF-89D1-57EEFDB34795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863543D8-B067-4ABA-B0F2-BE485DC2CE83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Users</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>Administrations</t>
-  </si>
-  <si>
-    <t>User_Administrations</t>
-  </si>
-  <si>
-    <t>Administrations_id</t>
   </si>
   <si>
     <t>category</t>
@@ -79,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,13 +84,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,11 +127,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -182,27 +164,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
-    <cellStyle name="Cálculo" xfId="4" builtinId="22"/>
-    <cellStyle name="Entrada" xfId="3" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Cálculo" xfId="3" builtinId="22"/>
+    <cellStyle name="Entrada" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -223,68 +202,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Conector recto de flecha 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BA67FCC-8226-4B17-AA35-DF57888ED613}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1952625" y="104775"/>
-          <a:ext cx="981075" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -298,9 +224,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5505450" y="104775"/>
-          <a:ext cx="476250" cy="9525"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2085975" y="95250"/>
+          <a:ext cx="3895725" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -595,7 +521,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,12 +532,6 @@
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
         <v>12</v>
@@ -632,15 +552,8 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
       <c r="K2" t="s">
         <v>1</v>
       </c>
@@ -656,33 +569,35 @@
       <c r="O2" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="3"/>
-      <c r="X2" s="4" t="s">
+      <c r="P2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="X3" s="5">
+      <c r="X3" s="4">
         <v>1</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="5"/>
+      <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="X4" s="5">
+      <c r="X4" s="4">
         <v>0</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="Y4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Z4" s="5"/>
+      <c r="Z4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>